<commit_message>
updated 14th July abbreviations
</commit_message>
<xml_diff>
--- a/abbreviations14thJuly.xlsx
+++ b/abbreviations14thJuly.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="23256" windowHeight="9936"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6919" uniqueCount="6250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6933" uniqueCount="6261">
   <si>
     <t>Abbreviation</t>
   </si>
@@ -18780,17 +18780,57 @@
   </si>
   <si>
     <t xml:space="preserve">a / o </t>
+  </si>
+  <si>
+    <t>geneva</t>
+  </si>
+  <si>
+    <t>Geneva</t>
+  </si>
+  <si>
+    <t>gibraltar</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>new delhi</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>houston</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>athens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Athens </t>
+  </si>
+  <si>
+    <t>venezuala</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -18910,18 +18950,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -18931,15 +18971,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -19160,10 +19201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3460"/>
+  <dimension ref="A1:C3467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2283" workbookViewId="0">
-      <selection activeCell="B2296" sqref="B2296"/>
+    <sheetView tabSelected="1" topLeftCell="A3445" workbookViewId="0">
+      <selection activeCell="B3459" sqref="B3459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -46856,6 +46897,62 @@
         <v>34</v>
       </c>
     </row>
+    <row r="3461" spans="1:2" ht="15" customHeight="1">
+      <c r="A3461" s="22" t="s">
+        <v>6250</v>
+      </c>
+      <c r="B3461" s="22" t="s">
+        <v>6251</v>
+      </c>
+    </row>
+    <row r="3462" spans="1:2" ht="15" customHeight="1">
+      <c r="A3462" s="22" t="s">
+        <v>6252</v>
+      </c>
+      <c r="B3462" s="22" t="s">
+        <v>6253</v>
+      </c>
+    </row>
+    <row r="3463" spans="1:2" ht="15" customHeight="1">
+      <c r="A3463" s="22" t="s">
+        <v>6254</v>
+      </c>
+      <c r="B3463" s="22" t="s">
+        <v>6255</v>
+      </c>
+    </row>
+    <row r="3464" spans="1:2" ht="15" customHeight="1">
+      <c r="A3464" s="22" t="s">
+        <v>6256</v>
+      </c>
+      <c r="B3464" s="22" t="s">
+        <v>6257</v>
+      </c>
+    </row>
+    <row r="3465" spans="1:2" ht="15" customHeight="1">
+      <c r="A3465" s="22" t="s">
+        <v>6258</v>
+      </c>
+      <c r="B3465" s="22" t="s">
+        <v>6259</v>
+      </c>
+    </row>
+    <row r="3466" spans="1:2" ht="15" customHeight="1">
+      <c r="A3466" s="22" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B3466" s="22" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="3467" spans="1:2" ht="15" customHeight="1">
+      <c r="A3467" s="22" t="s">
+        <v>6260</v>
+      </c>
+      <c r="B3467" s="22" t="s">
+        <v>1288</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A3:B3308">
     <sortCondition ref="A1209:A3308"/>

</xml_diff>

<commit_message>
Owners / Charterers problem fixed
</commit_message>
<xml_diff>
--- a/abbreviations14thJuly.xlsx
+++ b/abbreviations14thJuly.xlsx
@@ -19203,8 +19203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3467"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3445" workbookViewId="0">
-      <selection activeCell="B3459" sqref="B3459"/>
+    <sheetView tabSelected="1" topLeftCell="A3464" workbookViewId="0">
+      <selection activeCell="B3480" sqref="B3480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>